<commit_message>
add vehicle usage and assigned to in mass upload wtc
</commit_message>
<xml_diff>
--- a/FMS.Website/files_upload/csfWtcMassUpload.xlsx
+++ b/FMS.Website/files_upload/csfWtcMassUpload.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\vox\task\fms021020170830\hms-fms\FMS.Website\files_upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
   <si>
     <t>Manufacturer</t>
   </si>
@@ -54,6 +54,24 @@
   </si>
   <si>
     <t>white</t>
+  </si>
+  <si>
+    <t>Vehicle Usage</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>ASA</t>
+  </si>
+  <si>
+    <t>Formal Name 1</t>
+  </si>
+  <si>
+    <t>Formal Name 2</t>
+  </si>
+  <si>
+    <t>Formal Name 3</t>
   </si>
 </sst>
 </file>
@@ -372,19 +390,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -400,8 +420,14 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -417,8 +443,14 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -434,8 +466,14 @@
       <c r="E3" t="s">
         <v>9</v>
       </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -450,6 +488,12 @@
       </c>
       <c r="E4" t="s">
         <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>